<commit_message>
Incorporate feedback on UI.
</commit_message>
<xml_diff>
--- a/assets/DTT-Test-Hour-Log_Iurashchuk.xlsx
+++ b/assets/DTT-Test-Hour-Log_Iurashchuk.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <r>
       <rPr>
@@ -143,6 +143,49 @@
     <t xml:space="preserve">Organized and cleaned up the code.</t>
   </si>
   <si>
+    <t xml:space="preserve">Feedback incorporation. UI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed: distance values followed by “ km” at the overview and house detail screens; text style at the house detail screen; alignment of the text at the about screen; nested layouts eliminated; distance view is hidden when the device location is unknown.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feedback incorporation. UI. Fullscreen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed image shows as the background of the status bar. Had issue with system navigation at the bottom on APIs 30 and higher. Found solution with setting bottom system window inset to the house detail view separately.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feedback incorporation. UX</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Fixed the map to be responsive to the user gestures at the h</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ouse detail fragment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Total amount of hours</t>
   </si>
 </sst>
@@ -156,7 +199,7 @@
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <name val="Verdana"/>
@@ -230,6 +273,11 @@
       <name val="Open Sans"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Open Sans"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -435,11 +483,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -560,9 +608,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2219760</xdr:colOff>
+      <xdr:colOff>2219040</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>821880</xdr:rowOff>
+      <xdr:rowOff>821160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -576,7 +624,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="148320" y="131760"/>
-          <a:ext cx="2071440" cy="690120"/>
+          <a:ext cx="2070720" cy="689400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -598,8 +646,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -813,54 +861,101 @@
       <c r="E13" s="14"/>
       <c r="F13" s="15"/>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="9"/>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
+    <row r="14" s="16" customFormat="true" ht="37.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="21" t="n">
-        <f aca="false">SUMIF(E4:E13,"&lt;&gt;x",B4:B13)</f>
-        <v>20</v>
-      </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="9"/>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="23"/>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="9"/>
+      <c r="B14" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="12" t="n">
+        <v>44903</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15"/>
+    </row>
+    <row r="15" customFormat="false" ht="37.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" s="12" t="n">
+        <v>44903</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15"/>
+    </row>
+    <row r="16" customFormat="false" ht="37.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="12" t="n">
+        <v>44903</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="15"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="23"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="22"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="19"/>
       <c r="E17" s="20"/>
       <c r="F17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="24"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="27"/>
-    </row>
-    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="A18" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="21" t="n">
+        <f aca="false">SUMIF(E4:E17,"&lt;&gt;x",B4:B17)</f>
+        <v>24</v>
+      </c>
+      <c r="C18" s="20"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="23"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="9"/>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="23"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="9"/>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="24"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="27"/>
+    </row>
     <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Incorporate feedback on UX, format and logic.
</commit_message>
<xml_diff>
--- a/assets/DTT-Test-Hour-Log_Iurashchuk.xlsx
+++ b/assets/DTT-Test-Hour-Log_Iurashchuk.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <r>
       <rPr>
@@ -158,6 +158,15 @@
     <t xml:space="preserve">Feedback incorporation. UX</t>
   </si>
   <si>
+    <t xml:space="preserve">Fixed the map to be responsive to the user gestures at the house detail fragment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed: search being successful either on “1034ZH” or “1034 ZH”; pressing marker on the map goes immediately to the directions to the location at the house detail fragment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Feedback incorporation. Format and Logic</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="8"/>
@@ -165,7 +174,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Fixed the map to be responsive to the user gestures at the h</t>
+      <t xml:space="preserve">Fixed: all public funs and </t>
     </r>
     <r>
       <rPr>
@@ -173,7 +182,7 @@
         <rFont val="Open Sans"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">ouse detail fragment</t>
+      <t xml:space="preserve">vals/vars </t>
     </r>
     <r>
       <rPr>
@@ -182,7 +191,24 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">.</t>
+      <t xml:space="preserve">have javaDocs; all fun names start with a verb; const values are created for all strings and numbers; funs split up into private methods; the network request, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">the search functionality and database interactions perform</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Open Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the IO thread.</t>
     </r>
   </si>
   <si>
@@ -410,7 +436,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -480,6 +506,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -608,9 +638,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2219040</xdr:colOff>
+      <xdr:colOff>2218680</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>821160</xdr:rowOff>
+      <xdr:rowOff>820800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -624,7 +654,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="148320" y="131760"/>
-          <a:ext cx="2070720" cy="689400"/>
+          <a:ext cx="2070360" cy="689040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -646,7 +676,7 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -911,53 +941,83 @@
       </c>
       <c r="F16" s="15"/>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="9"/>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
+    <row r="17" customFormat="false" ht="37.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="12" t="n">
+        <v>44904</v>
+      </c>
+      <c r="D17" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="21" t="n">
-        <f aca="false">SUMIF(E4:E17,"&lt;&gt;x",B4:B17)</f>
-        <v>24</v>
-      </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="9"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="15"/>
+    </row>
+    <row r="18" customFormat="false" ht="37.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="C18" s="12" t="n">
+        <v>44904</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="23"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="20"/>
+      <c r="A19" s="19"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="21"/>
       <c r="F19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="23"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="20"/>
+      <c r="A20" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="22" t="n">
+        <f aca="false">SUMIF(E4:E19,"&lt;&gt;x",B4:B19)</f>
+        <v>29</v>
+      </c>
+      <c r="C20" s="21"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="21"/>
       <c r="F20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="24"/>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="27"/>
-    </row>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="24"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="25"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="26"/>
+      <c r="F23" s="28"/>
+    </row>
     <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>